<commit_message>
RDM-2314 Update CRUD in spreadsheet for new type.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V34_RDM-2314.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V34_RDM-2314.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="-5640" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="292">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -6920,10 +6920,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6931,7 +6931,7 @@
     <col min="1" max="1" width="33" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="11" width="14.5" style="1" customWidth="1"/>
     <col min="12" max="1025" width="8.83203125" customWidth="1"/>
   </cols>
@@ -7165,21 +7165,21 @@
       <c r="K10" s="97"/>
     </row>
     <row r="11" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="94">
-        <v>42736</v>
-      </c>
-      <c r="B11" s="95"/>
-      <c r="C11" s="96" t="s">
+      <c r="A11" s="138">
+        <v>42736</v>
+      </c>
+      <c r="B11" s="139"/>
+      <c r="C11" s="140" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="96" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="96" t="s">
-        <v>249</v>
-      </c>
-      <c r="F11" s="96" t="s">
-        <v>250</v>
+      <c r="D11" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="E11" s="140" t="s">
+        <v>253</v>
+      </c>
+      <c r="F11" s="140" t="s">
+        <v>258</v>
       </c>
       <c r="G11" s="95"/>
       <c r="H11" s="95"/>
@@ -7199,10 +7199,10 @@
         <v>54</v>
       </c>
       <c r="E12" s="96" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F12" s="96" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G12" s="95"/>
       <c r="H12" s="95"/>
@@ -7222,10 +7222,10 @@
         <v>54</v>
       </c>
       <c r="E13" s="96" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F13" s="96" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G13" s="95"/>
       <c r="H13" s="95"/>
@@ -7242,13 +7242,13 @@
         <v>24</v>
       </c>
       <c r="D14" s="96" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E14" s="96" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="F14" s="96" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="G14" s="95"/>
       <c r="H14" s="95"/>
@@ -7262,10 +7262,10 @@
       </c>
       <c r="B15" s="95"/>
       <c r="C15" s="96" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" s="96" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E15" s="96" t="s">
         <v>249</v>
@@ -7288,7 +7288,7 @@
         <v>27</v>
       </c>
       <c r="D16" s="96" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E16" s="96" t="s">
         <v>249</v>
@@ -7311,7 +7311,7 @@
         <v>27</v>
       </c>
       <c r="D17" s="96" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E17" s="96" t="s">
         <v>249</v>
@@ -7334,7 +7334,7 @@
         <v>27</v>
       </c>
       <c r="D18" s="96" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="E18" s="96" t="s">
         <v>249</v>
@@ -7357,7 +7357,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="96" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E19" s="96" t="s">
         <v>249</v>
@@ -7380,7 +7380,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="96" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E20" s="96" t="s">
         <v>249</v>
@@ -7403,7 +7403,7 @@
         <v>27</v>
       </c>
       <c r="D21" s="96" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E21" s="96" t="s">
         <v>249</v>
@@ -7426,7 +7426,7 @@
         <v>27</v>
       </c>
       <c r="D22" s="96" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E22" s="96" t="s">
         <v>249</v>
@@ -7449,7 +7449,7 @@
         <v>27</v>
       </c>
       <c r="D23" s="96" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E23" s="96" t="s">
         <v>249</v>
@@ -7472,7 +7472,7 @@
         <v>27</v>
       </c>
       <c r="D24" s="96" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E24" s="96" t="s">
         <v>249</v>
@@ -7495,7 +7495,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="96" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E25" s="96" t="s">
         <v>249</v>
@@ -7518,7 +7518,7 @@
         <v>27</v>
       </c>
       <c r="D26" s="96" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E26" s="96" t="s">
         <v>249</v>
@@ -7540,8 +7540,8 @@
       <c r="C27" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="98" t="s">
-        <v>96</v>
+      <c r="D27" s="96" t="s">
+        <v>93</v>
       </c>
       <c r="E27" s="96" t="s">
         <v>249</v>
@@ -7560,11 +7560,11 @@
         <v>42736</v>
       </c>
       <c r="B28" s="95"/>
-      <c r="C28" s="99" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="96" t="s">
-        <v>56</v>
+      <c r="C28" s="96" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="98" t="s">
+        <v>96</v>
       </c>
       <c r="E28" s="96" t="s">
         <v>249</v>
@@ -7586,8 +7586,8 @@
       <c r="C29" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="98" t="s">
-        <v>59</v>
+      <c r="D29" s="96" t="s">
+        <v>56</v>
       </c>
       <c r="E29" s="96" t="s">
         <v>249</v>
@@ -7602,17 +7602,27 @@
       <c r="K29" s="97"/>
     </row>
     <row r="30" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="81"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="26"/>
+      <c r="A30" s="94">
+        <v>42736</v>
+      </c>
+      <c r="B30" s="95"/>
+      <c r="C30" s="99" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="98" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="96" t="s">
+        <v>249</v>
+      </c>
+      <c r="F30" s="96" t="s">
+        <v>250</v>
+      </c>
+      <c r="G30" s="95"/>
+      <c r="H30" s="95"/>
+      <c r="I30" s="95"/>
+      <c r="J30" s="95"/>
+      <c r="K30" s="97"/>
     </row>
     <row r="31" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="81"/>
@@ -7839,7 +7849,7 @@
       <c r="A48" s="81"/>
       <c r="B48" s="17"/>
       <c r="C48" s="74"/>
-      <c r="D48" s="78"/>
+      <c r="D48" s="74"/>
       <c r="E48" s="74"/>
       <c r="F48" s="74"/>
       <c r="G48" s="17"/>
@@ -7851,8 +7861,8 @@
     <row r="49" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="81"/>
       <c r="B49" s="17"/>
-      <c r="C49" s="82"/>
-      <c r="D49" s="28"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="78"/>
       <c r="E49" s="74"/>
       <c r="F49" s="74"/>
       <c r="G49" s="17"/>
@@ -7865,7 +7875,7 @@
       <c r="A50" s="81"/>
       <c r="B50" s="17"/>
       <c r="C50" s="82"/>
-      <c r="D50" s="31"/>
+      <c r="D50" s="28"/>
       <c r="E50" s="74"/>
       <c r="F50" s="74"/>
       <c r="G50" s="17"/>
@@ -7878,7 +7888,7 @@
       <c r="A51" s="81"/>
       <c r="B51" s="17"/>
       <c r="C51" s="82"/>
-      <c r="D51" s="28"/>
+      <c r="D51" s="31"/>
       <c r="E51" s="74"/>
       <c r="F51" s="74"/>
       <c r="G51" s="17"/>
@@ -7888,17 +7898,30 @@
       <c r="K51" s="26"/>
     </row>
     <row r="52" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="83"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="78"/>
-      <c r="F52" s="78"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="37"/>
+      <c r="A52" s="81"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="26"/>
+    </row>
+    <row r="53" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="83"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="78"/>
+      <c r="F53" s="78"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
@@ -13193,7 +13216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -16889,7 +16912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
RDM-2416 Change READONLY to MANDATORY in import validation for OrderSummary type.
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V34_RDM-2314.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V34_RDM-2314.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5640" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -6922,7 +6922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -13216,7 +13216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -16913,7 +16913,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -17308,7 +17308,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="137" t="s">
-        <v>289</v>
+        <v>195</v>
       </c>
       <c r="L10" s="137"/>
       <c r="M10" s="137"/>

</xml_diff>